<commit_message>
after lesson, all commits combined since 16 Jan
</commit_message>
<xml_diff>
--- a/6_Webscraping/results/bom_rate.xlsx
+++ b/6_Webscraping/results/bom_rate.xlsx
@@ -25,118 +25,118 @@
     <t>EN</t>
   </si>
   <si>
-    <t>2,849.87</t>
-  </si>
-  <si>
-    <t>3,267.52</t>
-  </si>
-  <si>
-    <t>25.04</t>
-  </si>
-  <si>
-    <t>3,130.01</t>
-  </si>
-  <si>
-    <t>319.09</t>
-  </si>
-  <si>
-    <t>3,911.59</t>
-  </si>
-  <si>
-    <t>1,670.84</t>
-  </si>
-  <si>
-    <t>9.21</t>
-  </si>
-  <si>
-    <t>181.64</t>
-  </si>
-  <si>
-    <t>38.44</t>
-  </si>
-  <si>
-    <t>366.01</t>
-  </si>
-  <si>
-    <t>37.60</t>
-  </si>
-  <si>
-    <t>6.53</t>
-  </si>
-  <si>
-    <t>449.07</t>
-  </si>
-  <si>
-    <t>2.40</t>
-  </si>
-  <si>
-    <t>21.92</t>
-  </si>
-  <si>
-    <t>2,280.81</t>
-  </si>
-  <si>
-    <t>2,074.99</t>
-  </si>
-  <si>
-    <t>133.17</t>
-  </si>
-  <si>
-    <t>103.19</t>
-  </si>
-  <si>
-    <t>85.89</t>
+    <t>2,864.45</t>
+  </si>
+  <si>
+    <t>3,211.33</t>
+  </si>
+  <si>
+    <t>24.85</t>
+  </si>
+  <si>
+    <t>3,100.39</t>
+  </si>
+  <si>
+    <t>301.56</t>
+  </si>
+  <si>
+    <t>3,843.81</t>
+  </si>
+  <si>
+    <t>1,641.75</t>
+  </si>
+  <si>
+    <t>8.75</t>
+  </si>
+  <si>
+    <t>181.93</t>
+  </si>
+  <si>
+    <t>38.04</t>
+  </si>
+  <si>
+    <t>366.88</t>
+  </si>
+  <si>
+    <t>34.29</t>
+  </si>
+  <si>
+    <t>6.17</t>
+  </si>
+  <si>
+    <t>453.65</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
+    <t>22.03</t>
+  </si>
+  <si>
+    <t>2,240.48</t>
+  </si>
+  <si>
+    <t>2,064.41</t>
+  </si>
+  <si>
+    <t>129.49</t>
+  </si>
+  <si>
+    <t>102.32</t>
+  </si>
+  <si>
+    <t>88.02</t>
   </si>
   <si>
     <t>0.20</t>
   </si>
   <si>
-    <t>682.20</t>
-  </si>
-  <si>
-    <t>2,120.04</t>
-  </si>
-  <si>
-    <t>775.89</t>
-  </si>
-  <si>
-    <t>9,441.35</t>
-  </si>
-  <si>
-    <t>1,956.15</t>
-  </si>
-  <si>
-    <t>439.14</t>
-  </si>
-  <si>
-    <t>719.31</t>
-  </si>
-  <si>
-    <t>102.07</t>
-  </si>
-  <si>
-    <t>328.11</t>
-  </si>
-  <si>
-    <t>24.03</t>
-  </si>
-  <si>
-    <t>185.54</t>
-  </si>
-  <si>
-    <t>210.65</t>
+    <t>682.34</t>
+  </si>
+  <si>
+    <t>2,117.74</t>
+  </si>
+  <si>
+    <t>779.86</t>
+  </si>
+  <si>
+    <t>9,458.31</t>
+  </si>
+  <si>
+    <t>1,923.62</t>
+  </si>
+  <si>
+    <t>431.53</t>
+  </si>
+  <si>
+    <t>692.26</t>
+  </si>
+  <si>
+    <t>95.32</t>
+  </si>
+  <si>
+    <t>320.12</t>
+  </si>
+  <si>
+    <t>23.77</t>
+  </si>
+  <si>
+    <t>187.29</t>
+  </si>
+  <si>
+    <t>203.64</t>
   </si>
   <si>
     <t>0.13</t>
   </si>
   <si>
-    <t>5,206,081.39</t>
-  </si>
-  <si>
-    <t>66,145.48</t>
-  </si>
-  <si>
-    <t>4,010.87</t>
+    <t>5,480,967.53</t>
+  </si>
+  <si>
+    <t>69,760.82</t>
+  </si>
+  <si>
+    <t>3,993.57</t>
   </si>
   <si>
     <t>АНУ доллар</t>

</xml_diff>